<commit_message>
Inclusão de resultados de importância das variáveis
</commit_message>
<xml_diff>
--- a/src/Referencia_Variaveis/Variaveis_Utilizadas_ENEM.xlsx
+++ b/src/Referencia_Variaveis/Variaveis_Utilizadas_ENEM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Armazenamento\MBA\TCC\Entrega_4_TCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Armazenamento\MBA\TCC\TccMbaUspEsalq\src\Referencia_Variaveis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02BAF5A-178A-4AFE-8C99-83FD953FED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D5A478-F16A-470C-AEC2-58713D5FBEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52F243A9-C98F-4233-B92A-72B54D4FE366}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>BIN_Q023</t>
   </si>
   <si>
-    <t>BIN_Q024</t>
-  </si>
-  <si>
     <t>CAT_COR_RACA</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
     <t>CAT_CO_UF_ESC</t>
   </si>
   <si>
-    <t>CAT_TP_DEPENDENCIA_ADM_ESC</t>
-  </si>
-  <si>
     <t>CAT_ENSINO</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t>CAT_SIT_FUNC_ESC</t>
   </si>
   <si>
-    <t>CAT_LOCALIZACAO_ESCOLA</t>
-  </si>
-  <si>
     <t>NUM_NOTA_CH</t>
   </si>
   <si>
@@ -396,9 +387,6 @@
     <t>NUM_Q022</t>
   </si>
   <si>
-    <t>NUM_Q025</t>
-  </si>
-  <si>
     <t>Quantidade de geladeiras</t>
   </si>
   <si>
@@ -454,6 +442,18 @@
   </si>
   <si>
     <t>Binária</t>
+  </si>
+  <si>
+    <t>NUM_Q024</t>
+  </si>
+  <si>
+    <t>BIN_Q025</t>
+  </si>
+  <si>
+    <t>CAT_DEPENDENCIA_ADM_ESC</t>
+  </si>
+  <si>
+    <t>CAT_LOCALIZACAO_ESC</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,19 +828,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,13 +851,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,13 +868,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,13 +885,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,13 +902,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -919,13 +919,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -936,13 +936,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -950,16 +950,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -970,13 +970,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -984,16 +984,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,16 +1001,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,16 +1018,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1035,16 +1035,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,13 +1055,13 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,13 +1072,13 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,13 +1089,13 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,13 +1106,13 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,13 +1123,13 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,13 +1140,13 @@
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,13 +1157,13 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,10 +1177,10 @@
         <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1191,13 +1191,13 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,10 +1211,10 @@
         <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,13 +1225,13 @@
         <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,13 +1242,13 @@
         <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,13 +1259,13 @@
         <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,13 +1276,13 @@
         <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,16 +1290,16 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,13 +1310,13 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,13 +1327,13 @@
         <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,13 +1344,13 @@
         <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,13 +1361,13 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,16 +1375,16 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,13 +1395,13 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,13 +1412,13 @@
         <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,13 +1429,13 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E36" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,13 +1446,13 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,13 +1463,13 @@
         <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,16 +1477,16 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,13 +1497,13 @@
         <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1511,16 +1511,16 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C41" t="s">
         <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,10 +1534,10 @@
         <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,13 +1548,13 @@
         <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,10 +1568,10 @@
         <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E45" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,16 +1596,16 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E46" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>